<commit_message>
Corrigindo a leitura e tratamento da tabela e valores vazios
</commit_message>
<xml_diff>
--- a/criterios_por_ano.xlsx
+++ b/criterios_por_ano.xlsx
@@ -532,7 +532,7 @@
         <v>45.94</v>
       </c>
       <c r="G2" t="n">
-        <v>100</v>
+        <v>99.52</v>
       </c>
       <c r="H2" t="n">
         <v>89.95999999999999</v>
@@ -544,7 +544,7 @@
         <v>37.82</v>
       </c>
       <c r="K2" t="n">
-        <v>100</v>
+        <v>0.59</v>
       </c>
       <c r="L2" t="n">
         <v>1.18</v>
@@ -553,7 +553,7 @@
         <v>42.9</v>
       </c>
       <c r="N2" t="n">
-        <v>100</v>
+        <v>0.91</v>
       </c>
       <c r="O2" t="n">
         <v>70.98999999999999</v>
@@ -584,7 +584,7 @@
         <v>31.51</v>
       </c>
       <c r="G3" t="n">
-        <v>100</v>
+        <v>99.05</v>
       </c>
       <c r="H3" t="n">
         <v>83.33</v>
@@ -596,7 +596,7 @@
         <v>36.9</v>
       </c>
       <c r="K3" t="n">
-        <v>100</v>
+        <v>9.84</v>
       </c>
       <c r="L3" t="n">
         <v>6.03</v>
@@ -605,7 +605,7 @@
         <v>48.89</v>
       </c>
       <c r="N3" t="n">
-        <v>100</v>
+        <v>5.4</v>
       </c>
       <c r="O3" t="n">
         <v>64.84</v>
@@ -636,7 +636,7 @@
         <v>45.3</v>
       </c>
       <c r="G4" t="n">
-        <v>100</v>
+        <v>99.70999999999999</v>
       </c>
       <c r="H4" t="n">
         <v>80.90000000000001</v>
@@ -648,7 +648,7 @@
         <v>37.34</v>
       </c>
       <c r="K4" t="n">
-        <v>100</v>
+        <v>12.88</v>
       </c>
       <c r="L4" t="n">
         <v>12.59</v>
@@ -657,7 +657,7 @@
         <v>59.62</v>
       </c>
       <c r="N4" t="n">
-        <v>100</v>
+        <v>6.22</v>
       </c>
       <c r="O4" t="n">
         <v>70.77</v>
@@ -700,7 +700,7 @@
         <v>71.14</v>
       </c>
       <c r="K5" t="n">
-        <v>100</v>
+        <v>66.18000000000001</v>
       </c>
       <c r="L5" t="n">
         <v>69.68000000000001</v>
@@ -709,7 +709,7 @@
         <v>89.20999999999999</v>
       </c>
       <c r="N5" t="n">
-        <v>100</v>
+        <v>63.27</v>
       </c>
       <c r="O5" t="n">
         <v>92.42</v>

</xml_diff>